<commit_message>
Excel data read and Logging code update commit
</commit_message>
<xml_diff>
--- a/src/TestData/TestData.xlsx
+++ b/src/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rudrkrishna/PycharmProjects/seleniumAssessment/src/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C4863C-36A1-5946-93B3-CC90AD3D5B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACB7F93-40AF-C04C-AAFD-72705A7E4A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17380" xr2:uid="{33C62505-8A11-334F-AB78-58DEA2AF183C}"/>
   </bookViews>
@@ -61,13 +61,13 @@
     <t>searchitem3</t>
   </si>
   <si>
-    <t>Butter</t>
-  </si>
-  <si>
     <t>searchtest</t>
   </si>
   <si>
     <t>Besan</t>
+  </si>
+  <si>
+    <t>Milk</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,15 +478,15 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
manage address Functionality added
</commit_message>
<xml_diff>
--- a/src/TestData/TestData.xlsx
+++ b/src/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rudrkrishna/PycharmProjects/seleniumAssessment/src/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB283E62-900C-7548-866B-5CF6A7A58572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32268D8F-A905-2E46-A508-53E0929BAA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17380" xr2:uid="{33C62505-8A11-334F-AB78-58DEA2AF183C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>username</t>
   </si>
@@ -68,6 +68,30 @@
   </si>
   <si>
     <t>filtertest</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Naruto Uzumaki</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>locality</t>
+  </si>
+  <si>
+    <t>Konoha</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>D-no 11/a, Uzumaki Street, Hidden Leaf Village, Konoha</t>
   </si>
 </sst>
 </file>
@@ -430,15 +454,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1B15A4-606A-744D-A3A0-ECC3BCE5E22A}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -487,6 +512,46 @@
       </c>
       <c r="B6" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>9999999106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>500085</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Address Verification and Logout Functionalities are added
</commit_message>
<xml_diff>
--- a/src/TestData/TestData.xlsx
+++ b/src/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rudrkrishna/PycharmProjects/seleniumAssessment/src/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32268D8F-A905-2E46-A508-53E0929BAA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793F2884-D1B6-FA46-A95D-2E7CD604B37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17380" xr2:uid="{33C62505-8A11-334F-AB78-58DEA2AF183C}"/>
   </bookViews>
@@ -457,7 +457,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>